<commit_message>
mudancas nas funcoes e nos retornos dela
</commit_message>
<xml_diff>
--- a/Data/AtivosIbov.xlsx
+++ b/Data/AtivosIbov.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Risco\Novo Risco\pythonrisco\BBFinance\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{708FA1F8-B80C-4EE5-86FC-C81331DC3426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8203061-BC1A-4CB3-BE30-B67C932BCB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11835"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="IBOVDia_10-04-23" sheetId="1" r:id="rId1"/>
@@ -1453,12 +1453,12 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>3.5720000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0.214</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>0.19900000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>3.5630000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>3.7909999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>0.36899999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>3.1280000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>1.4139999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0.95099999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>0.183</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>0.629</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>0.97299999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>3.4550000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>0.309</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>0.95099999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>0.57899999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>1.7190000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>92</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>0.52800000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>104</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0.21099999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>0.59599999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0.85599999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>0.23300000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>2.3980000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>115</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>6.6130000000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1.075</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>119</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>121</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>126</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>0.85599999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>128</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>0.54600000000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>130</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>132</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>136</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0.38300000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>141</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>143</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>5.3250000000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>145</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>6.1840000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>146</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>1.651</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>148</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>150</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>152</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>1.6870000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>154</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>156</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>158</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>160</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>162</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>165</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>167</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>169</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>171</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>1.655</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>173</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>175</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>180</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>182</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>0.20399999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>186</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>14.701000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>188</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>192</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>2.8719999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>194</v>
       </c>
@@ -2971,10 +2971,10 @@
         <v>0.11799999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D92" s="2"/>
     </row>
   </sheetData>

</xml_diff>